<commit_message>
#129 named ranges support for fromJson and toJson integration tests
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/DataModelDto_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/DataModelDto_Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\spreadsheet_analytics\project\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spreadsheet\CalculationEngine\calculation-engine\engine-tests\engine-it\src\test\resources\datamodel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,10 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="My_Age">Sheet1!$C$1</definedName>
+    <definedName name="My_Id">Sheet1!$C$3</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -347,7 +351,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>